<commit_message>
Hide inactive tasks; Add forbidden students
</commit_message>
<xml_diff>
--- a/static/EnrollTaskData.xlsx
+++ b/static/EnrollTaskData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="課程" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="學生" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="禁止選課名單" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">課程名稱</t>
   </si>
@@ -45,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">身分證號</t>
+  </si>
+  <si>
+    <t xml:space="preserve">禁止原因</t>
   </si>
 </sst>
 </file>
@@ -59,6 +63,7 @@
       <sz val="10"/>
       <name val="文泉驛微米黑"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,12 +130,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -146,10 +151,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.64"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -180,14 +182,11 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.64"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -209,7 +208,48 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12頁 &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12頁 &amp;P</oddFooter>

</xml_diff>